<commit_message>
add: function playing song
</commit_message>
<xml_diff>
--- a/docs/_re_skin_asset.xlsx
+++ b/docs/_re_skin_asset.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROJECT_ANDROID\FROGOBOX\RELEASE\TEMPLATE-CODE\BaseMusicPlayer\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF841AB5-244A-4506-96D1-C5A240437755}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5554FAA5-3682-443C-8AC1-A081098361B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9495" yWindow="1440" windowWidth="10020" windowHeight="7875" xr2:uid="{EE5E1A3E-F3F9-48B6-8650-D84991C3A10B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EE5E1A3E-F3F9-48B6-8650-D84991C3A10B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,26 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>songImage (Image Cover)</t>
+  </si>
+  <si>
+    <t>songMusic (Music Title - Filename)</t>
+  </si>
+  <si>
+    <t>songName (Music Title)</t>
+  </si>
+  <si>
+    <t>artistName (Artist Name)</t>
+  </si>
+  <si>
+    <t>albumName (Album Name)</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -378,12 +398,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8EBFF7D-D20B-4BFB-AA6D-93FA55356B20}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="5" max="5" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>